<commit_message>
After validate refactor mdlScenario. TransferTblImportRows
</commit_message>
<xml_diff>
--- a/Code Plan.xlsx
+++ b/Code Plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Box Sync\Projects\Excel_Steps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40E1C3B4-B11B-4DBB-86F9-8B7E1D300FA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1248D077-66BC-4BF6-BEC2-103CB4F3A86E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38040" yWindow="277" windowWidth="26310" windowHeight="15316" xr2:uid="{BC6A1FF8-FCEF-4310-9430-53F13A45C0E8}"/>
+    <workbookView xWindow="0" yWindow="885" windowWidth="34898" windowHeight="15315" xr2:uid="{BC6A1FF8-FCEF-4310-9430-53F13A45C0E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="107">
   <si>
     <t>Arguments</t>
   </si>
@@ -180,15 +180,6 @@
 Provision and Refresh mdlDest</t>
   </si>
   <si>
-    <t>Sub</t>
-  </si>
-  <si>
-    <t>ResetRow</t>
-  </si>
-  <si>
-    <t>WriteToMdlDestAndSteps</t>
-  </si>
-  <si>
     <t>WriteRowToMdl</t>
   </si>
   <si>
@@ -199,23 +190,6 @@
   </si>
   <si>
     <t>WriteVarToMdlDest</t>
-  </si>
-  <si>
-    <t>R_MI,
-tblImp</t>
-  </si>
-  <si>
-    <t>mdlDest,
-R_MI,
-tblS</t>
-  </si>
-  <si>
-    <t>mdlDest|mdlScenario,
-R_MI|RowMdlImport</t>
-  </si>
-  <si>
-    <t>tblS|tblRowsCols,
-R_MI|RowMdlImport</t>
   </si>
   <si>
     <t>WriteRowToSteps</t>
@@ -237,12 +211,6 @@
     <t>Transfer ModelNew rows from mdlImport table to mdlDest</t>
   </si>
   <si>
-    <t>Reset mdlImportRow Class instance in loop over mdlImport rngMdl rows</t>
-  </si>
-  <si>
-    <t>Write mdlImportRow (R_MI instance) variables to mdl and ExcelSteps</t>
-  </si>
-  <si>
     <t>Write a mdlImport table row to destination Scenario Model</t>
   </si>
   <si>
@@ -294,9 +262,6 @@
   </si>
   <si>
     <t>Row-by-row transfer mdlDest to mdlImport Sheet</t>
-  </si>
-  <si>
-    <t>InitToTblWrite</t>
   </si>
   <si>
     <t>sGrpPrev|String,
@@ -379,18 +344,6 @@
 ModelDefnDest|String|ByVal</t>
   </si>
   <si>
-    <t>mdlDest|mdlScenario|ByVal,
-tblImp|tblRowsCols|ByRef,
-ModelNew|String|ByVal,
-R_MI|mdlImportRow|ByRef</t>
-  </si>
-  <si>
-    <t>mdlDest|mdlScenario|ByRef,
-tblImp|tblRowsCols|ByVal,
-tblS|tblRowsCols,
-rngMdl|String|ByVal</t>
-  </si>
-  <si>
     <t>mdlDest|mdlScenario|ByRef,
 rngMdl|Range|ByVal</t>
   </si>
@@ -473,43 +426,72 @@
   <si>
     <t xml:space="preserve"> Clear mdlDest region,
 ' Set rngMdl to tblImp rows whose Model col matches ModelNew
-' Set tblImp.rowCur to first rngMdl row</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> If new Group or SubGroup, write that heading and increment mdlDest.rowCur (.WriteGrpToMdlDest),
-' 'Write variable name, metadata and value (.WriteVarToMdlDest)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Write Grp to mdlDest rowCur,
-'Format the Grp string in mdlDest rowCur,
-' Increment mdlDest.rowCur to next row</t>
-  </si>
-  <si>
-    <t>Write variable's Description, Variable Name and Units to mdlDest</t>
-  </si>
-  <si>
-    <t>InitRead</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Set temp variables GrpPrev, SubGrpPrev and rngModel for R_MI.Grp, .SubGrp and .rngModel,
-' Re-instance mdlImportRow as R_MI,
-' R_MI.InitRead(Grp, SubGrp)
-' Set .rngModel to the temp variables</t>
-  </si>
-  <si>
-    <t>Set GrpPrev and SubGrpPrev attributes,
-'Write a mdlImport row to mdlDest (.WriteRowToMdl),
-'Write mdlImport row to tblS (WriteRowToSteps)</t>
-  </si>
-  <si>
-    <t>Write R_MI.sModel and .VarName to Steps rowCur,
-Write Step type Formula/Dropdown list name and Number Format,
-'Extend .rngRows to include new row and increment Steps tbl.rowCur</t>
-  </si>
-  <si>
-    <t>Set GrpPrev and SubGrpPrev attributes from temp variables,
-' Read the tblImp row and set Boolean flags based on the row's data,
-' Set the Step Type for the row (Col_Format, Col_Insert or Col_Dropdown)</t>
+' Set tblImp.rowCur to first rngMdl row
+' Instance R_MI Class as tblImportRow</t>
+  </si>
+  <si>
+    <t>R_MI|mdlImportRow|ByRef,
+mdlDest|mdlScenario|ByRef,
+tblImp|tblRowsCols|ByVal,
+tblS|tblRowsCols,</t>
+  </si>
+  <si>
+    <t>mdlDest|mdlScenario|ByVal,
+tblImp|tblRowsCols|ByRef,
+ModelNew|String|ByVal</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>InitToTblWrite</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Init</t>
+    </r>
+  </si>
+  <si>
+    <t>ReadRow</t>
+  </si>
+  <si>
+    <t>SetStepType</t>
+  </si>
+  <si>
+    <t>R_MI|mdlIMportRow|ByRef,
+tblImp|tblRowsCols|ByVal</t>
+  </si>
+  <si>
+    <t>R|Range</t>
+  </si>
+  <si>
+    <t>R_MI|mdlImportRow</t>
+  </si>
+  <si>
+    <t>mdlScenario. TransferTblImportRows</t>
+  </si>
+  <si>
+    <t>R_MI|RowMdlImport|ByVal,
+mdlDest|mdlScenario|ByVal</t>
+  </si>
+  <si>
+    <t>R_MI|RowMdlImport|ByVal,
+tblS|tblRowsCols|ByRef,</t>
+  </si>
+  <si>
+    <t>Read tblImport rowCur values</t>
   </si>
 </sst>
 </file>
@@ -565,14 +547,15 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -625,14 +608,26 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -684,7 +679,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="10">
+  <cellStyleXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -694,7 +689,9 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -719,9 +716,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -730,22 +724,25 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="6" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="8" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="8" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="9" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="9" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="11" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="11" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="10" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="10">
+  <cellStyles count="12">
+    <cellStyle name="20% - Accent2" xfId="10" builtinId="34"/>
     <cellStyle name="20% - Accent3" xfId="7" builtinId="38"/>
     <cellStyle name="40% - Accent2" xfId="6" builtinId="35"/>
+    <cellStyle name="40% - Accent4" xfId="11" builtinId="43"/>
     <cellStyle name="40% - Accent5" xfId="4" builtinId="47"/>
     <cellStyle name="60% - Accent2" xfId="9" builtinId="36"/>
     <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
@@ -1066,22 +1063,23 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B62ADAB2-59CA-4D89-A7D5-36DD0F6BBCE7}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D17" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H21" sqref="H21"/>
+      <selection pane="bottomRight" activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="21.3984375" customWidth="1"/>
+    <col min="1" max="1" width="20.59765625" customWidth="1"/>
     <col min="2" max="2" width="19.6640625" customWidth="1"/>
     <col min="3" max="3" width="26" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="58.1328125" style="1" hidden="1" customWidth="1"/>
-    <col min="5" max="6" width="14.6640625" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="58.1328125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" customWidth="1"/>
+    <col min="6" max="6" width="9.73046875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27.796875" style="1" customWidth="1"/>
     <col min="8" max="8" width="27.46484375" style="1" customWidth="1"/>
     <col min="9" max="9" width="52.1328125" style="1" customWidth="1"/>
@@ -1093,19 +1091,19 @@
         <v>5</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="12" t="s">
         <v>8</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>0</v>
@@ -1113,7 +1111,7 @@
       <c r="H1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="I1" s="12" t="s">
         <v>3</v>
       </c>
       <c r="J1" s="6" t="s">
@@ -1125,7 +1123,7 @@
         <v>9</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>9</v>
@@ -1136,7 +1134,7 @@
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="11" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="H2" s="11" t="s">
         <v>19</v>
@@ -1151,7 +1149,7 @@
         <v>9</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>10</v>
@@ -1161,7 +1159,7 @@
         <v>2</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="G3" s="11" t="s">
         <v>22</v>
@@ -1179,25 +1177,25 @@
         <v>9</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="H4" s="11"/>
-      <c r="I4" s="14"/>
+      <c r="I4" s="13"/>
       <c r="J4" s="3"/>
     </row>
     <row r="5" spans="1:10" ht="58.9" x14ac:dyDescent="0.45">
@@ -1205,22 +1203,22 @@
         <v>9</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>2</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="H5" s="11"/>
       <c r="I5" s="11"/>
@@ -1228,113 +1226,113 @@
     </row>
     <row r="6" spans="1:10" ht="35.65" x14ac:dyDescent="0.45">
       <c r="A6" s="8" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>2</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="I6" s="14"/>
+        <v>75</v>
+      </c>
+      <c r="I6" s="13"/>
       <c r="J6" s="3"/>
     </row>
     <row r="7" spans="1:10" ht="24" x14ac:dyDescent="0.45">
       <c r="A7" s="8" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>2</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="I7" s="14" t="s">
-        <v>55</v>
+        <v>82</v>
+      </c>
+      <c r="I7" s="13" t="s">
+        <v>46</v>
       </c>
       <c r="J7" s="3"/>
     </row>
     <row r="8" spans="1:10" ht="24" x14ac:dyDescent="0.45">
       <c r="A8" s="8" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="14" t="s">
-        <v>56</v>
+      <c r="D8" s="13" t="s">
+        <v>47</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>2</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="I8" s="14" t="s">
-        <v>56</v>
+        <v>83</v>
+      </c>
+      <c r="I8" s="13" t="s">
+        <v>47</v>
       </c>
       <c r="J8" s="3"/>
     </row>
     <row r="9" spans="1:10" ht="70.5" x14ac:dyDescent="0.45">
       <c r="A9" s="8" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>2</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="H9" s="11" t="s">
         <v>24</v>
@@ -1346,21 +1344,21 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10" s="8" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="H10" s="11"/>
       <c r="I10" s="11"/>
@@ -1368,34 +1366,34 @@
     </row>
     <row r="11" spans="1:10" ht="35.65" x14ac:dyDescent="0.45">
       <c r="A11" s="8" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="3" t="s">
         <v>2</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="H11" s="11"/>
-      <c r="I11" s="14"/>
+      <c r="I11" s="13"/>
       <c r="J11" s="3"/>
     </row>
     <row r="12" spans="1:10" ht="24" x14ac:dyDescent="0.45">
       <c r="A12" s="8" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>11</v>
@@ -1405,51 +1403,53 @@
         <v>2</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="H12" s="11"/>
-      <c r="I12" s="14" t="s">
+      <c r="I12" s="13" t="s">
         <v>15</v>
       </c>
       <c r="J12" s="3"/>
     </row>
     <row r="13" spans="1:10" ht="58.9" x14ac:dyDescent="0.45">
-      <c r="A13" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>98</v>
+      <c r="A13" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>86</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>2</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="H13" s="11"/>
-      <c r="I13" s="14"/>
+        <v>32</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="I13" s="13"/>
       <c r="J13" s="3"/>
     </row>
     <row r="14" spans="1:10" ht="47.25" x14ac:dyDescent="0.45">
-      <c r="A14" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="C14" s="16" t="s">
+      <c r="A14" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C14" s="15" t="s">
         <v>21</v>
       </c>
       <c r="D14" s="5" t="s">
@@ -1459,442 +1459,386 @@
         <v>2</v>
       </c>
       <c r="F14" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="H14" s="11"/>
+      <c r="I14" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="J14" s="3"/>
+    </row>
+    <row r="15" spans="1:10" ht="58.9" x14ac:dyDescent="0.45">
+      <c r="A15" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="I15" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="J15" s="3"/>
+    </row>
+    <row r="16" spans="1:10" ht="35.65" x14ac:dyDescent="0.45">
+      <c r="A16" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="I16" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="J16" s="3"/>
+    </row>
+    <row r="17" spans="1:10" ht="35.65" x14ac:dyDescent="0.45">
+      <c r="A17" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="G14" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="H14" s="11"/>
-      <c r="I14" s="22" t="s">
+      <c r="D17" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="I17" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="J17" s="3"/>
+    </row>
+    <row r="18" spans="1:10" ht="35.65" x14ac:dyDescent="0.45">
+      <c r="A18" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="J18" s="3"/>
+    </row>
+    <row r="19" spans="1:10" ht="35.65" x14ac:dyDescent="0.45">
+      <c r="A19" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E19" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="J19" s="3"/>
+    </row>
+    <row r="20" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A20" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E20" t="s">
+        <v>2</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="J20" s="3"/>
+    </row>
+    <row r="21" spans="1:10" ht="35.65" x14ac:dyDescent="0.45">
+      <c r="A21" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E21" t="s">
+        <v>2</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H21" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="I21" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="J21" s="3"/>
+    </row>
+    <row r="22" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A22" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="B22" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="J14" s="3"/>
-    </row>
-    <row r="15" spans="1:10" ht="58.9" x14ac:dyDescent="0.45">
-      <c r="A15" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="B15" s="15" t="s">
+      <c r="E22" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F22" s="21"/>
+      <c r="G22" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="H22" s="11"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="3"/>
+    </row>
+    <row r="23" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A23" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="B23" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="D23" s="5"/>
+      <c r="E23" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F23" s="21"/>
+      <c r="G23" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="H23" s="11"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="3"/>
+    </row>
+    <row r="24" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A24" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="B24" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F24" s="21"/>
+      <c r="G24" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="H24" s="11"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="3"/>
+    </row>
+    <row r="25" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A25" s="22" t="s">
         <v>103</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="G15" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="H15" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="I15" s="22" t="s">
+      <c r="B25" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F25" s="21"/>
+      <c r="G25" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="H25" s="11"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="3"/>
+    </row>
+    <row r="26" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A26" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="B26" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F26" s="21"/>
+      <c r="G26" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="H26" s="11"/>
+      <c r="I26" s="20"/>
+      <c r="J26" s="3"/>
+    </row>
+    <row r="27" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A27" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="B27" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="C27" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F27" s="21"/>
+      <c r="G27" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="H27" s="11"/>
+      <c r="I27" s="20"/>
+      <c r="J27" s="3"/>
+    </row>
+    <row r="28" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A28" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="B28" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F28" s="21"/>
+      <c r="G28" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="J15" s="3"/>
-    </row>
-    <row r="16" spans="1:10" ht="58.9" x14ac:dyDescent="0.45">
-      <c r="A16" s="21" t="s">
-        <v>103</v>
-      </c>
-      <c r="B16" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F16" s="19"/>
-      <c r="G16" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="H16" s="11"/>
-      <c r="I16" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="J16" s="3"/>
-    </row>
-    <row r="17" spans="1:10" ht="35.65" x14ac:dyDescent="0.45">
-      <c r="A17" s="21"/>
-      <c r="B17" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="22" t="s">
-        <v>114</v>
-      </c>
-      <c r="J17" s="3"/>
-    </row>
-    <row r="18" spans="1:10" ht="35.65" x14ac:dyDescent="0.45">
-      <c r="A18" s="21" t="s">
-        <v>103</v>
-      </c>
-      <c r="B18" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="C18" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F18" s="19"/>
-      <c r="G18" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="H18" s="11"/>
-      <c r="I18" s="22" t="s">
-        <v>112</v>
-      </c>
-      <c r="J18" s="3"/>
-    </row>
-    <row r="19" spans="1:10" ht="35.65" x14ac:dyDescent="0.45">
-      <c r="A19" s="21" t="s">
-        <v>103</v>
-      </c>
-      <c r="B19" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="C19" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F19" s="19"/>
-      <c r="G19" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="H19" s="11"/>
-      <c r="I19" s="22" t="s">
-        <v>107</v>
-      </c>
-      <c r="J19" s="3"/>
-    </row>
-    <row r="20" spans="1:10" ht="35.65" x14ac:dyDescent="0.45">
-      <c r="A20" s="21" t="s">
-        <v>103</v>
-      </c>
-      <c r="B20" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="C20" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F20" s="19"/>
-      <c r="G20" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="H20" s="11"/>
-      <c r="I20" s="22" t="s">
-        <v>108</v>
-      </c>
-      <c r="J20" s="3"/>
-    </row>
-    <row r="21" spans="1:10" ht="35.65" x14ac:dyDescent="0.45">
-      <c r="A21" s="21" t="s">
-        <v>103</v>
-      </c>
-      <c r="B21" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="C21" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F21" s="19"/>
-      <c r="G21" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="H21" s="11"/>
-      <c r="I21" s="24" t="s">
-        <v>113</v>
-      </c>
-      <c r="J21" s="3"/>
-    </row>
-    <row r="22" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A22" s="21" t="s">
-        <v>103</v>
-      </c>
-      <c r="B22" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="C22" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F22" s="19"/>
-      <c r="G22" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="H22" s="11"/>
-      <c r="I22" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="J22" s="3"/>
-    </row>
-    <row r="23" spans="1:10" ht="24" x14ac:dyDescent="0.45">
-      <c r="A23" s="21" t="s">
-        <v>103</v>
-      </c>
-      <c r="B23" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="C23" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F23" s="19"/>
-      <c r="G23" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="H23" s="11"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="3"/>
-    </row>
-    <row r="24" spans="1:10" ht="35.65" x14ac:dyDescent="0.45">
-      <c r="A24" s="21" t="s">
-        <v>103</v>
-      </c>
-      <c r="B24" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="C24" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="G24" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="H24" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="I24" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="J24" s="3"/>
-    </row>
-    <row r="25" spans="1:10" ht="35.65" x14ac:dyDescent="0.45">
-      <c r="A25" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="B25" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="E25" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="G25" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="H25" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="I25" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="J25" s="3"/>
-    </row>
-    <row r="26" spans="1:10" ht="35.65" x14ac:dyDescent="0.45">
-      <c r="A26" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="B26" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="E26" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="G26" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="H26" s="11"/>
-      <c r="I26" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="J26" s="3"/>
-    </row>
-    <row r="27" spans="1:10" ht="35.65" x14ac:dyDescent="0.45">
-      <c r="A27" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="B27" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="E27" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="G27" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="H27" s="11"/>
-      <c r="I27" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="J27" s="3"/>
-    </row>
-    <row r="28" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A28" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="B28" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="E28" t="s">
-        <v>2</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="G28" s="11" t="s">
-        <v>65</v>
-      </c>
       <c r="H28" s="11"/>
-      <c r="I28" s="11" t="s">
-        <v>75</v>
-      </c>
+      <c r="I28" s="20"/>
       <c r="J28" s="3"/>
-    </row>
-    <row r="29" spans="1:10" ht="35.65" x14ac:dyDescent="0.45">
-      <c r="A29" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="B29" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="E29" t="s">
-        <v>2</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="G29" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="H29" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="I29" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="J29" s="3"/>
-    </row>
-    <row r="30" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A30" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="B30" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="C30" s="3"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="F30" s="3"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
-      <c r="I30" s="11"/>
-      <c r="J30" s="3"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="I31" s="12"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="I32" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>